<commit_message>
Updates batch/fnbx tests for international environment and fixes some issues with test macros
</commit_message>
<xml_diff>
--- a/tests/batch.xlsx
+++ b/tests/batch.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\lr\finbox\excel-addin\tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="6855"/>
   </bookViews>
@@ -21,7 +16,6 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
     <definedName name="IQ_DAILY">500000</definedName>
@@ -38,6 +32,7 @@
     <definedName name="IQ_FWD_Q1" hidden="1">502</definedName>
     <definedName name="IQ_FWD_Q2" hidden="1">503</definedName>
     <definedName name="IQ_FY">1000</definedName>
+    <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_LATESTK" hidden="1">1000</definedName>
     <definedName name="IQ_LATESTQ" hidden="1">500</definedName>
     <definedName name="IQ_LTM">2000</definedName>
@@ -52,7 +47,7 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -167,9 +162,6 @@
     <t>ebitda</t>
   </si>
   <si>
-    <t>1/13/2016</t>
-  </si>
-  <si>
     <t>MT</t>
   </si>
   <si>
@@ -396,13 +388,16 @@
   </si>
   <si>
     <t>126 First Round</t>
+  </si>
+  <si>
+    <t>2016-01-13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -499,6 +494,10 @@
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,7 +517,6 @@
         <sz val="11"/>
         <color theme="0" tint="-0.34998626667073579"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -536,7 +534,6 @@
         <sz val="11"/>
         <color theme="0" tint="-0.34998626667073579"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -554,10 +551,10 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Sheet1"/>
+      <sheetName val="finboxio"/>
     </sheetNames>
     <definedNames>
       <definedName name="FNBX"/>
@@ -673,7 +670,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -725,7 +722,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -919,22 +916,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.42578125" customWidth="1"/>
     <col min="2" max="4" width="17.7109375" customWidth="1"/>
@@ -945,22 +942,22 @@
     <col min="9" max="9" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1"/>
+    <row r="3" spans="1:9">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -972,7 +969,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -986,7 +983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
@@ -1010,7 +1007,7 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
@@ -1030,7 +1027,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
@@ -1057,7 +1054,7 @@
         <v>42825</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="8" t="s">
         <v>18</v>
       </c>
@@ -1081,7 +1078,7 @@
         <v>42822</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
@@ -1104,10 +1101,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -1121,7 +1118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="8" t="s">
         <v>12</v>
       </c>
@@ -1145,7 +1142,7 @@
       </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
@@ -1169,7 +1166,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="8" t="s">
         <v>17</v>
       </c>
@@ -1183,7 +1180,7 @@
       </c>
       <c r="D14">
         <f ca="1">[1]!FNBX(LOWER('Cross-Sheet References'!A12),LEFT('Cross-Sheet References'!B14,5)&amp;"_price"&amp;"_close",'Cross-Sheet References'!D15)</f>
-        <v>123.28794110773545</v>
+        <v>133.35</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>21</v>
@@ -1196,7 +1193,7 @@
         <v>42767</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="8" t="s">
         <v>18</v>
       </c>
@@ -1220,7 +1217,7 @@
         <v>42802</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
@@ -1246,10 +1243,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1263,7 +1260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="8" t="s">
         <v>12</v>
       </c>
@@ -1287,7 +1284,7 @@
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="8" t="s">
         <v>14</v>
       </c>
@@ -1311,7 +1308,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="8" t="s">
         <v>17</v>
       </c>
@@ -1338,7 +1335,7 @@
         <v>42738</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="8" t="s">
         <v>18</v>
       </c>
@@ -1362,7 +1359,7 @@
         <v>42810</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="8" t="s">
         <v>13</v>
       </c>
@@ -1386,10 +1383,10 @@
       </c>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="2" t="s">
         <v>1</v>
       </c>
@@ -1403,7 +1400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="8" t="s">
         <v>12</v>
       </c>
@@ -1420,7 +1417,7 @@
         <v>Healthcare: Johnson &amp; Johnson, together with its subsidiaries, researches and develops, manufactures, and sells various products in the health care field worldwide. It operates through three segments: Consumer, Pharmaceutical, and Medical Devices. The Consumer segment offers baby care products under the JOHNSON’S brand; oral care products under the LISTERINE brand; beauty products under the AVEENO, CLEAN &amp; CLEAR, DABAO, JOHNSON’S Adult, LE PETITE MARSEILLAIS, NEUTROGENA, RoC, and OGX brands; over-the-counter medicines, including acetaminophen products under the TYLENOL brand; cold, flu, and allergy products under the SUDAFED brand; allergy products under the BENADRYL and ZYRTEC brands; ibuprofen products under the MOTRIN IB brand; and acid reflux products under the PEPCID brand. This segment also provides women’s health products, such as sanitary pads under the STAYFREE and CAREFREE brands, and tampons under the o.b. brand; wound care products comprising brand adhesive bandages under the BAND-AID brand and first aid products under the NEOSPORIN brand. The Pharmaceutical segment offers various products in the areas of immunology, infectious diseases and vaccines, neuroscience, oncology, and cardiovascular and metabolic diseases. The Medical Devices segment provides orthopaedic products; general surgery, biosurgical, endomechanical, and energy products; electrophysiology products to treat cardiovascular disease; sterilization and disinfection products to reduce surgical infection; diabetes care products that include blood glucose monitoring and insulin delivery products; and disposable contact lenses. The company markets its products to general public, retail outlets and distributors, wholesalers, hospitals, and health care professionals for prescription use, as well as for use in the professional fields by physicians, nurses, hospitals, eye care professionals, and clinics. Johnson &amp; Johnson was founded in 1885 and is based in New Brunswick, New Jersey.</v>
       </c>
       <c r="E26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>8</v>
@@ -1432,7 +1429,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="8" t="s">
         <v>14</v>
       </c>
@@ -1464,7 +1461,7 @@
         <v>FY-2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="8" t="s">
         <v>17</v>
       </c>
@@ -1484,14 +1481,14 @@
         <v>21</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="I28" s="7">
         <f>DATEVALUE(H28)</f>
         <v>42382</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="8" t="s">
         <v>18</v>
       </c>
@@ -1507,7 +1504,7 @@
         <f ca="1">IFERROR([1]!FNBX('Cross-Sheet References'!A26,'Cross-Sheet References'!B28,'Cross-Sheet References'!C29),[1]!FNBX('Cross-Sheet References'!A26,'Cross-Sheet References'!B28,'Cross-Sheet References'!C29-4))</f>
         <v>94.305497463586548</v>
       </c>
-      <c r="H29" s="10">
+      <c r="H29" s="14">
         <f>DATEVALUE(H28)+3</f>
         <v>42385</v>
       </c>
@@ -1516,7 +1513,7 @@
         <v>42385</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="8" t="s">
         <v>13</v>
       </c>
@@ -1533,7 +1530,7 @@
         <v>BX APO FIG</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>20</v>
@@ -1542,26 +1539,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="5"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" t="str">
         <f ca="1">LEFT([1]!FNBX([1]!FNBX("PG","benchmarks",1),"name"),12)</f>
@@ -1576,7 +1573,7 @@
         <v>CISCO SYSTEMS, INC.</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>20</v>
@@ -1585,9 +1582,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34" t="str">
         <f ca="1">[1]!FNBX("FINBOX:"&amp;[1]!FNBX("WFC","benchmarks",1),"sector")</f>
@@ -1602,13 +1599,13 @@
         <v>Industrials</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>32</v>
@@ -1617,9 +1614,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" t="str">
         <f ca="1">[1]!FNBX(CONCATENATE("FINBOX:",[1]!FNBX("WMT","benchmarks",1)),"sector")</f>
@@ -1634,19 +1631,19 @@
         <v>Healthcare</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" t="str">
         <f ca="1">[1]!FNBX([1]!FNBX("V","ticker")&amp;MID([1]!FNBX("AMZN","ticker"),3,1),"name")</f>
@@ -1661,21 +1658,21 @@
         <v>Citigroup Inc.</v>
       </c>
       <c r="F36" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G36" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G36" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="H36" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I36" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B37">
         <f ca="1">[1]!FNBX("AAPL","stock_price_close",[1]!FNBX("AAPL","period_end_date","FY"))</f>
@@ -1690,13 +1687,13 @@
         <v>81.438671763990357</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>21</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>25</v>
@@ -1705,9 +1702,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38">
         <f ca="1">[1]!FNBX("AAPL","stock_price_close",[1]!FNBX("AAPL","period_end_date","FY-1")-7)</f>
@@ -1725,9 +1722,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39">
         <f ca="1">[1]!FNBX("AAPL","stock_price_close",TEXT([1]!FNBX("AAPL","period_end_date","FY-2")-14,"YYYY-MM-DD"))</f>
@@ -1742,9 +1739,9 @@
         <v>73.540090776478067</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B40">
         <f ca="1">[1]!FNBX("AAPL","stock_price_close",DATE(YEAR([1]!FNBX("AAPL","period_end_date","FY-3")),MONTH([1]!FNBX("AAPL","period_end_date","FY-4")),12))</f>
@@ -1759,9 +1756,9 @@
         <v>72.060246057900841</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41">
         <f ca="1">[1]!FNBX([1]!FNBX([1]!FNBX("PEP","benchmarks",2),"benchmarks",1),"stock_price_close",DATE(YEAR([1]!FNBX([1]!FNBX("DIS","benchmarks",1),"period_end_date","FY-3")),MONTH([1]!FNBX("PEP","period_end_date","FY-4")),12))</f>
@@ -1776,18 +1773,19 @@
         <v>44.833809710775917</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="I41" s="15"/>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B43" s="3">
         <v>1</v>
@@ -1797,7 +1795,7 @@
       </c>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="4"/>
       <c r="B44">
         <f ca="1">[1]!FNBX("aapL","aP","fy-2")</f>
@@ -1808,10 +1806,10 @@
         <v>152.72054376402696</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="4"/>
       <c r="B45">
         <f ca="1">[1]!FNBX("AAPL","ap","FY-2")</f>
@@ -1826,29 +1824,29 @@
         <v>42879</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="4"/>
       <c r="C46">
         <f ca="1">[1]!FNBX("Aapl","stock_price_CLOSE",G46)</f>
         <v>152.72054376402696</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="4"/>
       <c r="C47">
         <f ca="1">[1]!FNBX("Aapl","stock_price_CLOSE",G47)</f>
         <v>152.72054376402696</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B49" s="3">
         <v>1</v>
@@ -1856,61 +1854,61 @@
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B50" t="e">
         <f>[1]!FNBX()</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B51" t="e">
         <f ca="1">[1]!FNBX(1,1,1)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B52" t="e">
         <f>[1]!FNBX(a)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B53" t="e">
         <f>[1]!FNBX("a")</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B54" t="e">
         <f>[1]!FNBX([1]!FNBX("bad"))</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B55">
         <f>IFERROR([1]!FNBX(),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" s="8"/>
     </row>
   </sheetData>
@@ -1920,7 +1918,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A3:H16"/>
   <sheetViews>
@@ -1928,7 +1926,7 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="54.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
@@ -1936,163 +1934,163 @@
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3">
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" t="s">
-        <v>90</v>
-      </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" t="s">
         <v>79</v>
       </c>
-      <c r="G4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5">
         <f ca="1">[1]!FNBX("AAPL","eps_basic")</f>
         <v>8.6280000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
         <v>81</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6">
+        <f ca="1">[1]!FNBX(Table1[ [#This Row],[AAPL] ],"eps_basic",Table1[ [#This Row],[Space Name] ])</f>
+        <v>6.4923999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" t="s">
         <v>82</v>
-      </c>
-      <c r="D6">
-        <f ca="1">[1]!FNBX(Table1[ [#This Row], [AAPL] ],"eps_basic",Table1[ [#This Row], [Space Name] ])</f>
-        <v>6.4923999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" t="s">
-        <v>83</v>
       </c>
       <c r="D7">
         <f ca="1">[1]!FNBX(CONCATENATE(Table1[[#Headers],[AAPL]],Table1[[#This Row],[AAPL]]),B5,Table1[[#This Row],[Space Name]])</f>
         <v>5.718</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8">
         <f ca="1">[1]!FNBX(Table1[[#This Row],[AAPL]],Table1[[#This Row],[Space Name]],E8)</f>
         <v>6.3776000000000002</v>
       </c>
       <c r="E8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9">
         <f ca="1">[1]!FNBX('Cross-Sheet References'!G12,'Cross-Sheet References'!H12,'Cross-Sheet References'!I12)</f>
         <v>4.0065999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10">
         <f ca="1">[1]!FNBX(Table2[[#This Row],[Column1]],Table2[[#This Row],[Space Name]],Table2[ [#This Row],[Column3] ])</f>
         <v>2.1105</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11">
         <f ca="1">[1]!FNBX(Table3[[#This Row],[Column1]],Table3[ [#This Row],[Space Name] ],Table3[[#This Row],[Column3]])</f>
         <v>1.7088000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
         <v>79</v>
       </c>
-      <c r="C13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" t="s">
-        <v>81</v>
-      </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F14" t="str">
         <f ca="1">Table4[[#Headers],[Column1]]&amp;": "&amp;[1]!FNBX(Table4[[#This Row],[Column1]],Table4[[#Headers],[eps_basic]]&amp;Table4[eps_basic],Table4[[#This Row],[Column3]])</f>
-        <v>Column1: 1.4323</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>Column1: 1,4323</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16">
         <f ca="1">[1]!FNBX(UPPER(Table5[[#This Row],[Column1]]),""&amp;Table5[[#This Row],[Space Name]]&amp;"_basic",CONCATENATE(Table5[[#This Row],[Column3]],Table5[[#This Row],[Column4]]-4))</f>
@@ -2110,48 +2108,48 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A3:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1"/>
       <c r="G3" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -2159,7 +2157,7 @@
       <c r="H5" s="4"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
@@ -2171,7 +2169,7 @@
       <c r="I6" s="9"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
@@ -2182,7 +2180,7 @@
       <c r="H7" s="4"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="B8" s="6"/>
       <c r="C8" s="6">
         <v>42822</v>
@@ -2190,7 +2188,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="B9" s="6" t="s">
         <v>20</v>
       </c>
@@ -2200,25 +2198,25 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -2226,16 +2224,16 @@
         <v>25</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="B13" s="6" t="s">
         <v>15</v>
       </c>
@@ -2243,7 +2241,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="B14" s="7" t="s">
         <v>21</v>
       </c>
@@ -2255,19 +2253,19 @@
         <v>42767</v>
       </c>
       <c r="G14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" t="s">
+        <v>89</v>
+      </c>
+      <c r="I14" t="s">
         <v>79</v>
       </c>
-      <c r="H14" t="s">
-        <v>90</v>
-      </c>
-      <c r="I14" t="s">
-        <v>80</v>
-      </c>
       <c r="J14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="B15" s="6"/>
       <c r="C15" s="6">
         <v>42802</v>
@@ -2277,7 +2275,7 @@
         <v>03/08/17</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="4" t="str">
         <f>LEFT('Batch Tests'!F16,1)</f>
         <v>A</v>
@@ -2291,24 +2289,24 @@
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
@@ -2317,7 +2315,7 @@
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>16</v>
@@ -2326,7 +2324,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
@@ -2334,12 +2332,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="C22" s="6">
         <v>42810</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="4" t="s">
         <v>30</v>
       </c>
@@ -2350,12 +2348,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
@@ -2366,7 +2364,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
         <v>33</v>
@@ -2383,23 +2381,23 @@
         <v>FY-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="B28" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="10">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="C29" s="14">
         <f>DATEVALUE(C28)+3</f>
         <v>42385</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>20</v>
@@ -2408,14 +2406,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>20</v>
@@ -2424,15 +2422,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>32</v>
@@ -2441,41 +2439,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C35" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>25</v>
@@ -2484,23 +2482,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="D38" s="4">
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:5">
       <c r="E45" s="6"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2517,7 +2515,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2525,19 +2523,19 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="78.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix duplicate keys in batch test workbook
</commit_message>
<xml_diff>
--- a/tests/batch.xlsx
+++ b/tests/batch.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\lr\finbox\excel-addin\tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="6855"/>
   </bookViews>
@@ -16,6 +21,7 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
+    <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
     <definedName name="IQ_DAILY">500000</definedName>
@@ -32,7 +38,6 @@
     <definedName name="IQ_FWD_Q1" hidden="1">502</definedName>
     <definedName name="IQ_FWD_Q2" hidden="1">503</definedName>
     <definedName name="IQ_FY">1000</definedName>
-    <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_LATESTK" hidden="1">1000</definedName>
     <definedName name="IQ_LATESTQ" hidden="1">500</definedName>
     <definedName name="IQ_LTM">2000</definedName>
@@ -47,7 +52,7 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -207,9 +212,6 @@
     <t>3-level multi</t>
   </si>
   <si>
-    <t>MRK</t>
-  </si>
-  <si>
     <t>bench</t>
   </si>
   <si>
@@ -231,18 +233,12 @@
     <t>AMGN</t>
   </si>
   <si>
-    <t>MMM</t>
-  </si>
-  <si>
     <t>period_end_date</t>
   </si>
   <si>
     <t>ORCL</t>
   </si>
   <si>
-    <t>BAC</t>
-  </si>
-  <si>
     <t>INTC</t>
   </si>
   <si>
@@ -391,13 +387,22 @@
   </si>
   <si>
     <t>2016-01-13</t>
+  </si>
+  <si>
+    <t>AIG</t>
+  </si>
+  <si>
+    <t>MPX</t>
+  </si>
+  <si>
+    <t>BLL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,7 +556,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="finboxio"/>
@@ -916,22 +921,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" customWidth="1"/>
     <col min="2" max="4" width="17.7109375" customWidth="1"/>
@@ -942,22 +947,22 @@
     <col min="9" max="9" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1"/>
-    <row r="3" spans="1:9">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -969,7 +974,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -983,13 +988,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B5">
         <f ca="1">[1]!FNBX("AAPL","revenue")</f>
-        <v>220457</v>
+        <v>223507</v>
       </c>
       <c r="C5">
         <f ca="1">[1]!FNBX(F5,G5)</f>
@@ -997,7 +1002,7 @@
       </c>
       <c r="D5">
         <f ca="1">[1]!FNBX('Cross-Sheet References'!A5,'Cross-Sheet References'!B6)</f>
-        <v>72174</v>
+        <v>72531</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>8</v>
@@ -1007,7 +1012,7 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
@@ -1027,7 +1032,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
@@ -1041,7 +1046,7 @@
       </c>
       <c r="D7">
         <f ca="1">[1]!FNBX('Cross-Sheet References'!A5,'Cross-Sheet References'!B7,'Cross-Sheet References'!C7)</f>
-        <v>123.73499649450807</v>
+        <v>122.95068169632374</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>21</v>
@@ -1054,7 +1059,7 @@
         <v>42825</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>18</v>
       </c>
@@ -1068,7 +1073,7 @@
       </c>
       <c r="D8">
         <f ca="1">[1]!FNBX('Cross-Sheet References'!A5,'Cross-Sheet References'!B7,'Cross-Sheet References'!C8)</f>
-        <v>124.83773311521384</v>
+        <v>124.04642843805735</v>
       </c>
       <c r="H8" s="6">
         <v>42822</v>
@@ -1078,7 +1083,7 @@
         <v>42822</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
@@ -1101,10 +1106,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -1118,13 +1123,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B12">
         <f ca="1">[1]!FNBX(UPPER("AAPL"),LOWER("da"))</f>
-        <v>10393</v>
+        <v>10221</v>
       </c>
       <c r="C12">
         <f ca="1">[1]!FNBX(""&amp;F12,UPPER(G12))</f>
@@ -1132,7 +1137,7 @@
       </c>
       <c r="D12">
         <f ca="1">[1]!FNBX(LEFT('Cross-Sheet References'!A12,LEN('Cross-Sheet References'!A12)),UPPER('Cross-Sheet References'!B13))</f>
-        <v>3775</v>
+        <v>4025</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>8</v>
@@ -1142,7 +1147,7 @@
       </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
@@ -1166,7 +1171,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>17</v>
       </c>
@@ -1180,7 +1185,7 @@
       </c>
       <c r="D14">
         <f ca="1">[1]!FNBX(LOWER('Cross-Sheet References'!A12),LEFT('Cross-Sheet References'!B14,5)&amp;"_price"&amp;"_close",'Cross-Sheet References'!D15)</f>
-        <v>133.35</v>
+        <v>122.50646004426959</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>21</v>
@@ -1193,7 +1198,7 @@
         <v>42767</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>18</v>
       </c>
@@ -1207,7 +1212,7 @@
       </c>
       <c r="D15">
         <f ca="1">[1]!FNBX(LOWER('Cross-Sheet References'!A12),LEFT('Cross-Sheet References'!B14,5)&amp;"_price"&amp;"_close",'Cross-Sheet References'!D14/1)</f>
-        <v>111.76057270216607</v>
+        <v>111.05215977528847</v>
       </c>
       <c r="H15" s="6">
         <v>42802</v>
@@ -1217,7 +1222,7 @@
         <v>42802</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
@@ -1243,10 +1248,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1260,7 +1265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>12</v>
       </c>
@@ -1284,7 +1289,7 @@
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>14</v>
       </c>
@@ -1308,7 +1313,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>17</v>
       </c>
@@ -1322,7 +1327,7 @@
       </c>
       <c r="D21">
         <f ca="1">-[1]!FNBX('Cross-Sheet References'!A19,'Cross-Sheet References'!B21,'Cross-Sheet References'!C21)*2</f>
-        <v>-228.67340354709739</v>
+        <v>-227.22391925054168</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>21</v>
@@ -1335,7 +1340,7 @@
         <v>42738</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>18</v>
       </c>
@@ -1349,7 +1354,7 @@
       </c>
       <c r="D22">
         <f ca="1">IFERROR(12/0,[1]!FNBX('Cross-Sheet References'!A19,'Cross-Sheet References'!B21,'Cross-Sheet References'!C22))</f>
-        <v>127.61941107735453</v>
+        <v>126.81047427306102</v>
       </c>
       <c r="H22" s="6">
         <v>42810</v>
@@ -1359,7 +1364,7 @@
         <v>42810</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>13</v>
       </c>
@@ -1383,10 +1388,10 @@
       </c>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>1</v>
       </c>
@@ -1400,7 +1405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>12</v>
       </c>
@@ -1429,7 +1434,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>14</v>
       </c>
@@ -1461,7 +1466,7 @@
         <v>FY-2</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>17</v>
       </c>
@@ -1475,20 +1480,20 @@
       </c>
       <c r="D28">
         <f ca="1">[1]!FNBX('Cross-Sheet References'!A26,'Cross-Sheet References'!B28,'Cross-Sheet References'!C28)-[1]!FNBX('Cross-Sheet References'!A26,LEFT('Cross-Sheet References'!B28,LEN("stock_price"))&amp;"_open",'Cross-Sheet References'!C28)</f>
-        <v>-1.4111266416069981</v>
+        <v>-1.402181981337236</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>21</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I28" s="7">
         <f>DATEVALUE(H28)</f>
         <v>42382</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>18</v>
       </c>
@@ -1502,7 +1507,7 @@
       </c>
       <c r="D29">
         <f ca="1">IFERROR([1]!FNBX('Cross-Sheet References'!A26,'Cross-Sheet References'!B28,'Cross-Sheet References'!C29),[1]!FNBX('Cross-Sheet References'!A26,'Cross-Sheet References'!B28,'Cross-Sheet References'!C29-4))</f>
-        <v>94.305497463586548</v>
+        <v>93.707726426238125</v>
       </c>
       <c r="H29" s="14">
         <f>DATEVALUE(H28)+3</f>
@@ -1513,7 +1518,7 @@
         <v>42385</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>13</v>
       </c>
@@ -1539,10 +1544,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
@@ -1556,7 +1561,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>39</v>
       </c>
@@ -1566,14 +1571,14 @@
       </c>
       <c r="C33" t="str">
         <f ca="1">UPPER([1]!FNBX([1]!FNBX(F33,G33,IF(I33&gt;0,I33,1)),H33))</f>
-        <v>BRISTOL-MYERS SQUIBB COMPANY</v>
+        <v>THE TRAVELERS COMPANIES, INC.</v>
       </c>
       <c r="D33" t="str">
         <f ca="1">UPPER([1]!FNBX([1]!FNBX('Cross-Sheet References'!A33,'Cross-Sheet References'!B33,IF('Cross-Sheet References'!D33&gt;0,'Cross-Sheet References'!D33,1)),'Cross-Sheet References'!C33))</f>
         <v>CISCO SYSTEMS, INC.</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>20</v>
@@ -1582,7 +1587,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>43</v>
       </c>
@@ -1599,13 +1604,13 @@
         <v>Industrials</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>32</v>
@@ -1614,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>40</v>
       </c>
@@ -1631,17 +1636,17 @@
         <v>Healthcare</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>44</v>
       </c>
@@ -1658,19 +1663,19 @@
         <v>Citigroup Inc.</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I36" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>42</v>
       </c>
@@ -1693,7 +1698,7 @@
         <v>21</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>25</v>
@@ -1702,7 +1707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>45</v>
       </c>
@@ -1722,7 +1727,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>41</v>
       </c>
@@ -1739,7 +1744,7 @@
         <v>73.540090776478067</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>46</v>
       </c>
@@ -1756,36 +1761,36 @@
         <v>72.060246057900841</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B41">
         <f ca="1">[1]!FNBX([1]!FNBX([1]!FNBX("PEP","benchmarks",2),"benchmarks",1),"stock_price_close",DATE(YEAR([1]!FNBX([1]!FNBX("DIS","benchmarks",1),"period_end_date","FY-3")),MONTH([1]!FNBX("PEP","period_end_date","FY-4")),12))</f>
-        <v>73.579096611452457</v>
+        <v>73.068284893353024</v>
       </c>
       <c r="C41">
         <f ca="1">[1]!FNBX([1]!FNBX([1]!FNBX(F41,G33,2),G33,J34),G37,DATE(YEAR([1]!FNBX([1]!FNBX(G41,G33,1),H37,CONCATENATE(I37,I38-2))),MONTH([1]!FNBX(F41,H37,I37&amp;(I38-3))),J37))</f>
-        <v>16.718314826544777</v>
+        <v>51.23</v>
       </c>
       <c r="D41">
         <f ca="1">[1]!FNBX([1]!FNBX([1]!FNBX('Cross-Sheet References'!A41,'Cross-Sheet References'!B33,2),'Cross-Sheet References'!B33,'Cross-Sheet References'!E34),'Cross-Sheet References'!B37,DATE(YEAR([1]!FNBX([1]!FNBX('Cross-Sheet References'!B41,'Cross-Sheet References'!B33,1),'Cross-Sheet References'!C37,CONCATENATE('Cross-Sheet References'!D37,'Cross-Sheet References'!D38-2))),MONTH([1]!FNBX('Cross-Sheet References'!A41,'Cross-Sheet References'!C37,'Cross-Sheet References'!D37&amp;('Cross-Sheet References'!D38-3))),'Cross-Sheet References'!E37))</f>
-        <v>44.833809710775917</v>
+        <v>46.282696618418392</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I41" s="15"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B43" s="3">
         <v>1</v>
@@ -1795,7 +1800,7 @@
       </c>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44">
         <f ca="1">[1]!FNBX("aapL","aP","fy-2")</f>
@@ -1806,10 +1811,10 @@
         <v>152.72054376402696</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45">
         <f ca="1">[1]!FNBX("AAPL","ap","FY-2")</f>
@@ -1824,29 +1829,29 @@
         <v>42879</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="C46">
         <f ca="1">[1]!FNBX("Aapl","stock_price_CLOSE",G46)</f>
         <v>152.72054376402696</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="C47">
         <f ca="1">[1]!FNBX("Aapl","stock_price_CLOSE",G47)</f>
         <v>152.72054376402696</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B49" s="3">
         <v>1</v>
@@ -1854,61 +1859,61 @@
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B50" t="e">
         <f>[1]!FNBX()</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B51" t="e">
         <f ca="1">[1]!FNBX(1,1,1)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B52" t="e">
         <f>[1]!FNBX(a)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B53" t="e">
         <f>[1]!FNBX("a")</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B54" t="e">
         <f>[1]!FNBX([1]!FNBX("bad"))</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B55">
         <f>IFERROR([1]!FNBX(),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
     </row>
   </sheetData>
@@ -1918,7 +1923,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A3:H16"/>
   <sheetViews>
@@ -1926,7 +1931,7 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
@@ -1934,167 +1939,167 @@
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3">
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
         <v>80</v>
-      </c>
-      <c r="C4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" t="s">
-        <v>89</v>
-      </c>
-      <c r="H4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" t="s">
-        <v>83</v>
       </c>
       <c r="D5">
         <f ca="1">[1]!FNBX("AAPL","eps_basic")</f>
-        <v>8.6280000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>8.8736000000000033</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D6">
         <f ca="1">[1]!FNBX(Table1[ [#This Row],[AAPL] ],"eps_basic",Table1[ [#This Row],[Space Name] ])</f>
         <v>6.4923999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D7">
         <f ca="1">[1]!FNBX(CONCATENATE(Table1[[#Headers],[AAPL]],Table1[[#This Row],[AAPL]]),B5,Table1[[#This Row],[Space Name]])</f>
         <v>5.718</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
         <v>80</v>
-      </c>
-      <c r="C8" t="s">
-        <v>83</v>
       </c>
       <c r="D8">
         <f ca="1">[1]!FNBX(Table1[[#This Row],[AAPL]],Table1[[#This Row],[Space Name]],E8)</f>
         <v>6.3776000000000002</v>
       </c>
       <c r="E8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D9">
         <f ca="1">[1]!FNBX('Cross-Sheet References'!G12,'Cross-Sheet References'!H12,'Cross-Sheet References'!I12)</f>
         <v>4.0065999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D10">
         <f ca="1">[1]!FNBX(Table2[[#This Row],[Column1]],Table2[[#This Row],[Space Name]],Table2[ [#This Row],[Column3] ])</f>
-        <v>2.1105</v>
+        <v>1.6778999999999999</v>
       </c>
       <c r="F10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" t="s">
         <v>80</v>
       </c>
-      <c r="G10" t="s">
-        <v>83</v>
-      </c>
       <c r="H10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D11">
         <f ca="1">[1]!FNBX(Table3[[#This Row],[Column1]],Table3[ [#This Row],[Space Name] ],Table3[[#This Row],[Column3]])</f>
-        <v>1.7088000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>3.3765000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F14" t="str">
         <f ca="1">Table4[[#Headers],[Column1]]&amp;": "&amp;[1]!FNBX(Table4[[#This Row],[Column1]],Table4[[#Headers],[eps_basic]]&amp;Table4[eps_basic],Table4[[#This Row],[Column3]])</f>
-        <v>Column1: 1,4323</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>Column1: 1.7088</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B16">
         <f ca="1">[1]!FNBX(UPPER(Table5[[#This Row],[Column1]]),""&amp;Table5[[#This Row],[Space Name]]&amp;"_basic",CONCATENATE(Table5[[#This Row],[Column3]],Table5[[#This Row],[Column4]]-4))</f>
-        <v>1.9069999999999998</v>
+        <v>1.4322999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2108,7 +2113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A3:J48"/>
   <sheetViews>
@@ -2116,7 +2121,7 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
@@ -2127,29 +2132,29 @@
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="G3" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -2157,7 +2162,7 @@
       <c r="H5" s="4"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
@@ -2169,7 +2174,7 @@
       <c r="I6" s="9"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
@@ -2180,7 +2185,7 @@
       <c r="H7" s="4"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="6">
         <v>42822</v>
@@ -2188,7 +2193,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>20</v>
       </c>
@@ -2198,25 +2203,25 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="I11" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -2224,16 +2229,16 @@
         <v>25</v>
       </c>
       <c r="G12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="I12" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>15</v>
       </c>
@@ -2241,7 +2246,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>21</v>
       </c>
@@ -2253,19 +2258,19 @@
         <v>42767</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="6">
         <v>42802</v>
@@ -2275,7 +2280,7 @@
         <v>03/08/17</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f>LEFT('Batch Tests'!F16,1)</f>
         <v>A</v>
@@ -2289,24 +2294,24 @@
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I16" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
@@ -2315,7 +2320,7 @@
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>16</v>
@@ -2324,7 +2329,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
@@ -2332,12 +2337,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" s="6">
         <v>42810</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>30</v>
       </c>
@@ -2348,12 +2353,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
@@ -2364,7 +2369,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
         <v>33</v>
@@ -2381,21 +2386,21 @@
         <v>FY-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C29" s="14">
         <f>DATEVALUE(C28)+3</f>
         <v>42385</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>35</v>
       </c>
@@ -2406,14 +2411,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>20</v>
@@ -2422,15 +2427,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>32</v>
@@ -2439,41 +2444,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C35" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>25</v>
@@ -2482,23 +2487,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D38" s="4">
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E45" s="6"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2515,7 +2520,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2523,17 +2528,17 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="78.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>

</xml_diff>